<commit_message>
I don't know what changed here, but something has apperently.
</commit_message>
<xml_diff>
--- a/all.xlsx
+++ b/all.xlsx
@@ -1366,8 +1366,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="286293352"/>
-        <c:axId val="286292960"/>
+        <c:axId val="232300360"/>
+        <c:axId val="303592240"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -1501,7 +1501,7 @@
                 </c:marker>
                 <c:cat>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>all!$B$59:$F$59</c15:sqref>
@@ -1585,7 +1585,7 @@
                 </c:marker>
                 <c:cat>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>all!$B$59:$F$59</c15:sqref>
@@ -1669,7 +1669,7 @@
                 </c:marker>
                 <c:cat>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>all!$B$59:$F$59</c15:sqref>
@@ -1755,7 +1755,7 @@
                 </c:marker>
                 <c:cat>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>all!$B$59:$F$59</c15:sqref>
@@ -1838,7 +1838,7 @@
                 </c:marker>
                 <c:cat>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>all!$B$59:$F$59</c15:sqref>
@@ -1918,7 +1918,7 @@
                 </c:marker>
                 <c:cat>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>all!$B$59:$F$59</c15:sqref>
@@ -1998,7 +1998,7 @@
                 </c:marker>
                 <c:cat>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>all!$B$59:$F$59</c15:sqref>
@@ -2079,7 +2079,7 @@
                 </c:marker>
                 <c:cat>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>all!$B$59:$F$59</c15:sqref>
@@ -2160,7 +2160,7 @@
                 </c:marker>
                 <c:cat>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>all!$B$59:$F$59</c15:sqref>
@@ -2241,7 +2241,7 @@
                 </c:marker>
                 <c:cat>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>all!$B$59:$F$59</c15:sqref>
@@ -2322,7 +2322,7 @@
                 </c:marker>
                 <c:cat>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>all!$B$59:$F$59</c15:sqref>
@@ -2402,7 +2402,7 @@
                 </c:marker>
                 <c:cat>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>all!$B$59:$F$59</c15:sqref>
@@ -2482,7 +2482,7 @@
                 </c:marker>
                 <c:cat>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>all!$B$59:$F$59</c15:sqref>
@@ -2562,7 +2562,7 @@
                 </c:marker>
                 <c:cat>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>all!$B$59:$F$59</c15:sqref>
@@ -2642,7 +2642,7 @@
                 </c:marker>
                 <c:cat>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>all!$B$59:$F$59</c15:sqref>
@@ -2692,7 +2692,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="286293352"/>
+        <c:axId val="232300360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2735,7 +2735,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="286292960"/>
+        <c:crossAx val="303592240"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2743,7 +2743,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="286292960"/>
+        <c:axId val="303592240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="160"/>
@@ -2795,7 +2795,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="286293352"/>
+        <c:crossAx val="232300360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="10"/>
@@ -3000,7 +3000,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -3062,11 +3061,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="286292176"/>
-        <c:axId val="286291784"/>
+        <c:axId val="303586248"/>
+        <c:axId val="303586632"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="286292176"/>
+        <c:axId val="303586248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3109,7 +3108,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="286291784"/>
+        <c:crossAx val="303586632"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3117,7 +3116,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="286291784"/>
+        <c:axId val="303586632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3168,7 +3167,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="286292176"/>
+        <c:crossAx val="303586248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3324,11 +3323,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="286291000"/>
-        <c:axId val="286290608"/>
+        <c:axId val="304405616"/>
+        <c:axId val="304406000"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="286291000"/>
+        <c:axId val="304405616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3371,7 +3370,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="286290608"/>
+        <c:crossAx val="304406000"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3379,7 +3378,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="286290608"/>
+        <c:axId val="304406000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3430,7 +3429,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="286291000"/>
+        <c:crossAx val="304405616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3867,11 +3866,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="291780336"/>
-        <c:axId val="291779160"/>
+        <c:axId val="232123960"/>
+        <c:axId val="232125136"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="291780336"/>
+        <c:axId val="232123960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3914,7 +3913,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="291779160"/>
+        <c:crossAx val="232125136"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3922,7 +3921,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="291779160"/>
+        <c:axId val="232125136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3973,7 +3972,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="291780336"/>
+        <c:crossAx val="232123960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4421,11 +4420,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="292162096"/>
-        <c:axId val="352380336"/>
+        <c:axId val="304648664"/>
+        <c:axId val="304649056"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="292162096"/>
+        <c:axId val="304648664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4468,7 +4467,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="352380336"/>
+        <c:crossAx val="304649056"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4476,7 +4475,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="352380336"/>
+        <c:axId val="304649056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4527,7 +4526,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="292162096"/>
+        <c:crossAx val="304648664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7456,16 +7455,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>818028</xdr:colOff>
-      <xdr:row>62</xdr:row>
-      <xdr:rowOff>34736</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>638734</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>68354</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>560294</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>840442</xdr:colOff>
       <xdr:row>88</xdr:row>
-      <xdr:rowOff>100851</xdr:rowOff>
+      <xdr:rowOff>33618</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -7486,16 +7485,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>655543</xdr:colOff>
-      <xdr:row>62</xdr:row>
-      <xdr:rowOff>12326</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>935690</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>101973</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>806823</xdr:colOff>
-      <xdr:row>85</xdr:row>
-      <xdr:rowOff>168087</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>481853</xdr:colOff>
+      <xdr:row>88</xdr:row>
+      <xdr:rowOff>89647</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -7782,8 +7781,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L58" sqref="L58"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A44" sqref="A44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9195,7 +9194,7 @@
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" t="str">
-        <f t="shared" ref="A29:A53" si="1">"Threads: "&amp;B3&amp;" "&amp;C3</f>
+        <f t="shared" ref="A29:A51" si="1">"Threads: "&amp;B3&amp;" "&amp;C3</f>
         <v>Threads: 1 Simd128</v>
       </c>
       <c r="B29" s="1">
@@ -9529,7 +9528,7 @@
         <v>0.67834034819774225</v>
       </c>
       <c r="I37" s="6">
-        <f t="shared" ref="I37:I51" si="9">(($G$28-G37)/$G$28)</f>
+        <f t="shared" ref="I37" si="9">(($G$28-G37)/$G$28)</f>
         <v>0.67834034819774225</v>
       </c>
     </row>
@@ -9567,7 +9566,7 @@
         <v>0.68048920539641378</v>
       </c>
       <c r="I38" s="2">
-        <f t="shared" ref="I38:I51" si="10">(($G$29-G38)/$G$29)</f>
+        <f t="shared" ref="I38" si="10">(($G$29-G38)/$G$29)</f>
         <v>0.67059699488569091</v>
       </c>
     </row>
@@ -9605,7 +9604,7 @@
         <v>0.69004954802962226</v>
       </c>
       <c r="I39" s="2">
-        <f t="shared" ref="I39:I51" si="11">(($G$30-G39)/$G$30)</f>
+        <f t="shared" ref="I39" si="11">(($G$30-G39)/$G$30)</f>
         <v>0.65853642630284925</v>
       </c>
     </row>
@@ -9643,7 +9642,7 @@
         <v>0.62747222172891248</v>
       </c>
       <c r="I40" s="6">
-        <f t="shared" ref="I40:I51" si="12">(($G$28-G40)/$G$28)</f>
+        <f t="shared" ref="I40" si="12">(($G$28-G40)/$G$28)</f>
         <v>0.62747222172891248</v>
       </c>
     </row>
@@ -9681,7 +9680,7 @@
         <v>0.63858944988071764</v>
       </c>
       <c r="I41" s="2">
-        <f t="shared" ref="I41:I51" si="13">(($G$29-G41)/$G$29)</f>
+        <f t="shared" ref="I41" si="13">(($G$29-G41)/$G$29)</f>
         <v>0.62740000244119765</v>
       </c>
     </row>
@@ -9757,7 +9756,7 @@
         <v>0.66016089790264421</v>
       </c>
       <c r="I43" s="6">
-        <f t="shared" ref="I43:I51" si="14">(($G$28-G43)/$G$28)</f>
+        <f t="shared" ref="I43" si="14">(($G$28-G43)/$G$28)</f>
         <v>0.66016089790264421</v>
       </c>
     </row>
@@ -9795,7 +9794,7 @@
         <v>0.67201809065454299</v>
       </c>
       <c r="I44" s="2">
-        <f t="shared" ref="I44:I51" si="15">(($G$29-G44)/$G$29)</f>
+        <f t="shared" ref="I44" si="15">(($G$29-G44)/$G$29)</f>
         <v>0.66186361028720686</v>
       </c>
     </row>
@@ -9833,7 +9832,7 @@
         <v>0.68011034352116595</v>
       </c>
       <c r="I45" s="2">
-        <f t="shared" ref="I45:I51" si="16">(($G$30-G45)/$G$30)</f>
+        <f t="shared" ref="I45" si="16">(($G$30-G45)/$G$30)</f>
         <v>0.64758668814441389</v>
       </c>
     </row>
@@ -9871,7 +9870,7 @@
         <v>0.68234799647184874</v>
       </c>
       <c r="I46" s="6">
-        <f t="shared" ref="I46:I51" si="17">(($G$28-G46)/$G$28)</f>
+        <f t="shared" ref="I46" si="17">(($G$28-G46)/$G$28)</f>
         <v>0.68234799647184874</v>
       </c>
     </row>
@@ -9909,7 +9908,7 @@
         <v>0.69087238866492617</v>
       </c>
       <c r="I47" s="2">
-        <f t="shared" ref="I47:I51" si="18">(($G$29-G47)/$G$29)</f>
+        <f t="shared" ref="I47" si="18">(($G$29-G47)/$G$29)</f>
         <v>0.681301646587816</v>
       </c>
     </row>
@@ -9947,7 +9946,7 @@
         <v>0.71422567144387816</v>
       </c>
       <c r="I48" s="2">
-        <f t="shared" ref="I48:I51" si="19">(($G$30-G48)/$G$30)</f>
+        <f t="shared" ref="I48" si="19">(($G$30-G48)/$G$30)</f>
         <v>0.68517057200806075</v>
       </c>
     </row>
@@ -9985,7 +9984,7 @@
         <v>0.67591918402623619</v>
       </c>
       <c r="I49" s="6">
-        <f t="shared" ref="I49:I51" si="20">(($G$28-G49)/$G$28)</f>
+        <f t="shared" ref="I49" si="20">(($G$28-G49)/$G$28)</f>
         <v>0.67591918402623619</v>
       </c>
     </row>
@@ -10023,7 +10022,7 @@
         <v>0.66876224641413162</v>
       </c>
       <c r="I50" s="2">
-        <f t="shared" ref="I50:I51" si="21">(($G$29-G50)/$G$29)</f>
+        <f t="shared" ref="I50" si="21">(($G$29-G50)/$G$29)</f>
         <v>0.65850696351630111</v>
       </c>
     </row>

</xml_diff>